<commit_message>
"improving findind desired elements, excel manipulation"
</commit_message>
<xml_diff>
--- a/today_orders.xlsx
+++ b/today_orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgnieszkaMędrek\Documents\UiPath\Lunch to choice automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA653AF-4F64-420C-8BF0-38497B0F7102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBFA034-B7D1-4115-AF42-3BC8CB4FA1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="525" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10_45" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>comapny adres</t>
   </si>
@@ -39,112 +39,16 @@
     <t>comment</t>
   </si>
   <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>order close time</t>
+  </si>
+  <si>
     <t>order code</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pilotów 10  </t>
-  </si>
-  <si>
-    <t>dziś 12:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> kuchnia 12 piętro, Creadis </t>
-  </si>
-  <si>
-    <t>CRE62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nowy lunch 02 </t>
-  </si>
-  <si>
-    <t>CRE38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nowy lunch 04 </t>
-  </si>
-  <si>
-    <t>CRE309</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sos teriyaki </t>
-  </si>
-  <si>
-    <t>CRE183</t>
-  </si>
-  <si>
-    <t>Sos teriyaki</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aleja Pokoju 18C m. 18C </t>
-  </si>
-  <si>
-    <t>dziś 13:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Biuro-recepcja II piętro  </t>
-  </si>
-  <si>
-    <t>P4437</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nowy lunch 03 </t>
-  </si>
-  <si>
-    <t>P4436</t>
-  </si>
-  <si>
-    <t>Nowy lunch 06</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> aleja 29 Listopada 20  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Przedsionek IV piętro </t>
-  </si>
-  <si>
-    <t>BRAI25</t>
-  </si>
-  <si>
-    <t>Tempura bento</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wadowicka 3a  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4 piętro,stolik w sali Kogel Mogel </t>
-  </si>
-  <si>
-    <t>HAVI100</t>
-  </si>
-  <si>
-    <t>Nowy lunch 02</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kotlarska 11  </t>
-  </si>
-  <si>
-    <t>dziś 13:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Recepcja - 4 piętro </t>
-  </si>
-  <si>
-    <t>CF100</t>
-  </si>
-  <si>
-    <t>CF140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wege set </t>
-  </si>
-  <si>
-    <t>CF35</t>
-  </si>
-  <si>
-    <t>Yaki tokugawa</t>
-  </si>
-  <si>
-    <t>index</t>
   </si>
 </sst>
 </file>
@@ -179,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -483,17 +388,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.5546875" customWidth="1"/>
     <col min="2" max="2" width="40.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="18.77734375" customWidth="1"/>
     <col min="5" max="5" width="25.77734375" customWidth="1"/>
     <col min="6" max="6" width="25.5546875" customWidth="1"/>
@@ -511,237 +416,32 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -750,13 +450,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97BFB14C-8EBC-4992-A71C-4CC0904D441D}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -769,17 +472,41 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -791,7 +518,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,10 +542,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>

</xml_diff>